<commit_message>
add annotation for performer
</commit_message>
<xml_diff>
--- a/Calculate-Total-Cost-Performer/Data/Invoices.xlsx
+++ b/Calculate-Total-Cost-Performer/Data/Invoices.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cd12d7bc64581e5/Documents/UiPath/Calculate-Total-Cost-Bot/Calculate-Total-Cost-Performer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P15\Documents\UiPath\Calculate-Total-Cost\Calculate-Total-Cost-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{93909F7A-C44A-4A06-BA42-9D5AF9ED2155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DCA9279-B754-4184-A471-1B217CE85B23}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8002A5-79FC-4A5A-BD62-4818750C2700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="9420" xr2:uid="{8F1C72BF-2C56-41AD-89A9-DC15E2BA2B20}"/>
+    <workbookView xWindow="10728" yWindow="2820" windowWidth="12312" windowHeight="9420" xr2:uid="{09F9C20C-53FB-447F-B91D-8FF60BDA9470}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>PDF_File_Name</t>
   </si>
@@ -48,82 +59,124 @@
     <t>GrandTotal</t>
   </si>
   <si>
-    <t>Invoice 001</t>
-  </si>
-  <si>
-    <t>Customer B</t>
-  </si>
-  <si>
-    <t>Invoice 002</t>
-  </si>
-  <si>
-    <t>Customer C</t>
-  </si>
-  <si>
-    <t>Invoice 003</t>
-  </si>
-  <si>
-    <t>Customer D</t>
-  </si>
-  <si>
-    <t>Invoice 004</t>
-  </si>
-  <si>
-    <t>Customer E</t>
-  </si>
-  <si>
-    <t>Invoice 005</t>
-  </si>
-  <si>
-    <t>Customer F</t>
-  </si>
-  <si>
-    <t>Invoice 006</t>
-  </si>
-  <si>
-    <t>Customer A</t>
-  </si>
-  <si>
-    <t>Invoice 007</t>
-  </si>
-  <si>
-    <t>Invoice 008</t>
-  </si>
-  <si>
-    <t>Invoice 009</t>
-  </si>
-  <si>
-    <t>Invoice 010</t>
-  </si>
-  <si>
-    <t>Invoice 011</t>
-  </si>
-  <si>
-    <t>Invoice 012</t>
-  </si>
-  <si>
-    <t>Invoice 013</t>
-  </si>
-  <si>
-    <t>Invoice 014</t>
-  </si>
-  <si>
-    <t>Invoice 015</t>
-  </si>
-  <si>
-    <t>Invoice 016</t>
-  </si>
-  <si>
-    <t>Invoice 017</t>
-  </si>
-  <si>
-    <t>Invoice 018</t>
-  </si>
-  <si>
-    <t>Invoice 019</t>
-  </si>
-  <si>
-    <t>Invoice 020</t>
+    <t>Invoice 109.pdf</t>
+  </si>
+  <si>
+    <t>Ram Farndell</t>
+  </si>
+  <si>
+    <t>Invoice 110.pdf</t>
+  </si>
+  <si>
+    <t>Keri Wreiford</t>
+  </si>
+  <si>
+    <t>Invoice 111.pdf</t>
+  </si>
+  <si>
+    <t>Orville Gerhardt</t>
+  </si>
+  <si>
+    <t>Invoice 112.pdf</t>
+  </si>
+  <si>
+    <t>Hamilton Skouling</t>
+  </si>
+  <si>
+    <t>Invoice 113.pdf</t>
+  </si>
+  <si>
+    <t>Garwin Slorach</t>
+  </si>
+  <si>
+    <t>Invoice 114.pdf</t>
+  </si>
+  <si>
+    <t>Boony Dumper</t>
+  </si>
+  <si>
+    <t>Invoice 115.pdf</t>
+  </si>
+  <si>
+    <t>Dulci Scay</t>
+  </si>
+  <si>
+    <t>Invoice 116.pdf</t>
+  </si>
+  <si>
+    <t>Keri Dancy</t>
+  </si>
+  <si>
+    <t>Invoice 117.pdf</t>
+  </si>
+  <si>
+    <t>Hamel Pavic</t>
+  </si>
+  <si>
+    <t>Invoice 118.pdf</t>
+  </si>
+  <si>
+    <t>Yancy Bulbrook</t>
+  </si>
+  <si>
+    <t>Invoice 119.pdf</t>
+  </si>
+  <si>
+    <t>Stirling Grunwald</t>
+  </si>
+  <si>
+    <t>Invoice 120.pdf</t>
+  </si>
+  <si>
+    <t>Wye Caseri</t>
+  </si>
+  <si>
+    <t>Invoice 121.pdf</t>
+  </si>
+  <si>
+    <t>Noby Everington</t>
+  </si>
+  <si>
+    <t>Invoice 122.pdf</t>
+  </si>
+  <si>
+    <t>Zorina Conibere</t>
+  </si>
+  <si>
+    <t>Invoice 123.pdf</t>
+  </si>
+  <si>
+    <t>Bridie Farbrace</t>
+  </si>
+  <si>
+    <t>Invoice 124.pdf</t>
+  </si>
+  <si>
+    <t>Zenia Beals</t>
+  </si>
+  <si>
+    <t>Invoice 125.pdf</t>
+  </si>
+  <si>
+    <t>Lynelle Vischi</t>
+  </si>
+  <si>
+    <t>Invoice 126.pdf</t>
+  </si>
+  <si>
+    <t>Jaquelyn De</t>
+  </si>
+  <si>
+    <t>Invoice 127.pdf</t>
+  </si>
+  <si>
+    <t>Dal Cremins</t>
+  </si>
+  <si>
+    <t>Invoice 128.pdf</t>
+  </si>
+  <si>
+    <t>Krissy Linney</t>
   </si>
 </sst>
 </file>
@@ -134,7 +187,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -143,7 +196,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -175,7 +227,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,39 +256,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -288,7 +340,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -399,13 +451,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -414,6 +459,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -478,31 +530,51 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9507428-5FFF-425D-A418-6410BED4C3F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A8DB93-7D33-4594-B371-1626844A8EC6}">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -533,22 +605,22 @@
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>45567</v>
+        <v>42652</v>
       </c>
       <c r="C2">
-        <v>1001</v>
+        <v>6604</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2">
-        <v>102</v>
+        <v>2000</v>
       </c>
       <c r="F2">
-        <v>64</v>
+        <v>375</v>
       </c>
       <c r="G2">
-        <v>166</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -556,22 +628,22 @@
         <v>9</v>
       </c>
       <c r="B3" s="1">
-        <v>45568</v>
+        <v>42757</v>
       </c>
       <c r="C3">
-        <v>1002</v>
+        <v>3152</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>156</v>
+        <v>1400</v>
       </c>
       <c r="F3">
-        <v>102</v>
+        <v>300</v>
       </c>
       <c r="G3">
-        <v>258</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -579,22 +651,22 @@
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>45569</v>
+        <v>43184</v>
       </c>
       <c r="C4">
-        <v>1003</v>
+        <v>6374</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4">
-        <v>212</v>
+        <v>1200</v>
       </c>
       <c r="F4">
-        <v>144</v>
+        <v>675</v>
       </c>
       <c r="G4">
-        <v>356</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -602,22 +674,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>45570</v>
+        <v>43396</v>
       </c>
       <c r="C5">
-        <v>1004</v>
+        <v>9020</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5">
-        <v>270</v>
+        <v>1200</v>
       </c>
       <c r="F5">
-        <v>38</v>
+        <v>450</v>
       </c>
       <c r="G5">
-        <v>308</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -625,22 +697,22 @@
         <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>45571</v>
+        <v>42696</v>
       </c>
       <c r="C6">
-        <v>1005</v>
+        <v>7008</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="E6">
-        <v>55</v>
+        <v>600</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>300</v>
       </c>
       <c r="G6">
-        <v>135</v>
+        <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -648,22 +720,22 @@
         <v>17</v>
       </c>
       <c r="B7" s="1">
-        <v>45572</v>
+        <v>43130</v>
       </c>
       <c r="C7">
-        <v>1006</v>
+        <v>5352</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7">
-        <v>112</v>
+        <v>400</v>
       </c>
       <c r="F7">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="G7">
-        <v>238</v>
+        <v>475</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -671,325 +743,324 @@
         <v>19</v>
       </c>
       <c r="B8" s="1">
-        <v>45573</v>
+        <v>42671</v>
       </c>
       <c r="C8">
-        <v>1007</v>
+        <v>5255</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>171</v>
+        <v>1400</v>
       </c>
       <c r="F8">
-        <v>176</v>
+        <v>600</v>
       </c>
       <c r="G8">
-        <v>347</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
-        <v>45574</v>
+        <v>42665</v>
       </c>
       <c r="C9">
-        <v>1008</v>
+        <v>5402</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E9">
-        <v>232</v>
+        <v>1000</v>
       </c>
       <c r="F9">
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="G9">
-        <v>278</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1">
-        <v>45575</v>
+        <v>42632</v>
       </c>
       <c r="C10">
-        <v>1009</v>
+        <v>1443</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E10">
-        <v>295</v>
+        <v>1600</v>
       </c>
       <c r="F10">
-        <v>96</v>
+        <v>375</v>
       </c>
       <c r="G10">
-        <v>391</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1">
-        <v>45576</v>
+        <v>42600</v>
       </c>
       <c r="C11">
-        <v>1010</v>
+        <v>5298</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>60</v>
+        <v>800</v>
       </c>
       <c r="F11">
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="G11">
-        <v>210</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
-        <v>45577</v>
+        <v>42891</v>
       </c>
       <c r="C12">
-        <v>1011</v>
+        <v>6357</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E12">
-        <v>122</v>
+        <v>400</v>
       </c>
       <c r="F12">
-        <v>208</v>
+        <v>750</v>
       </c>
       <c r="G12">
-        <v>330</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1">
-        <v>45578</v>
+        <v>42664</v>
       </c>
       <c r="C13">
-        <v>1012</v>
+        <v>3893</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E13">
-        <v>186</v>
+        <v>400</v>
       </c>
       <c r="F13">
-        <v>54</v>
+        <v>525</v>
       </c>
       <c r="G13">
-        <v>240</v>
+        <v>925</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1">
-        <v>45579</v>
+        <v>42483</v>
       </c>
       <c r="C14">
-        <v>1013</v>
+        <v>7260</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E14">
-        <v>252</v>
+        <v>2000</v>
       </c>
       <c r="F14">
-        <v>112</v>
+        <v>300</v>
       </c>
       <c r="G14">
-        <v>364</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1">
-        <v>45580</v>
+        <v>42946</v>
       </c>
       <c r="C15">
-        <v>1014</v>
+        <v>2381</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E15">
-        <v>320</v>
+        <v>1600</v>
       </c>
       <c r="F15">
-        <v>174</v>
+        <v>450</v>
       </c>
       <c r="G15">
-        <v>494</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1">
-        <v>45581</v>
+        <v>43094</v>
       </c>
       <c r="C16">
-        <v>1015</v>
+        <v>5542</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E16">
-        <v>65</v>
+        <v>1000</v>
       </c>
       <c r="F16">
-        <v>240</v>
+        <v>525</v>
       </c>
       <c r="G16">
-        <v>305</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1">
-        <v>45582</v>
+        <v>43434</v>
       </c>
       <c r="C17">
-        <v>1016</v>
+        <v>8437</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E17">
-        <v>132</v>
+        <v>1400</v>
       </c>
       <c r="F17">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="G17">
-        <v>194</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1">
-        <v>45583</v>
+        <v>42386</v>
       </c>
       <c r="C18">
-        <v>1017</v>
+        <v>7354</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E18">
-        <v>201</v>
+        <v>1600</v>
       </c>
       <c r="F18">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="G18">
-        <v>329</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1">
-        <v>45584</v>
+        <v>42425</v>
       </c>
       <c r="C19">
-        <v>1018</v>
+        <v>5424</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="E19">
-        <v>272</v>
+        <v>1400</v>
       </c>
       <c r="F19">
-        <v>198</v>
+        <v>600</v>
       </c>
       <c r="G19">
-        <v>470</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1">
-        <v>45585</v>
+        <v>43054</v>
       </c>
       <c r="C20">
-        <v>1019</v>
+        <v>8179</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E20">
-        <v>345</v>
+        <v>1600</v>
       </c>
       <c r="F20">
-        <v>272</v>
+        <v>450</v>
       </c>
       <c r="G20">
-        <v>617</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1">
-        <v>45586</v>
+        <v>43249</v>
       </c>
       <c r="C21">
-        <v>1020</v>
+        <v>7189</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E21">
-        <v>70</v>
+        <v>1000</v>
       </c>
       <c r="F21">
-        <v>70</v>
+        <v>525</v>
       </c>
       <c r="G21">
-        <v>140</v>
+        <v>1525</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add condition for cleaning up
</commit_message>
<xml_diff>
--- a/Calculate-Total-Cost-Performer/Data/Invoices.xlsx
+++ b/Calculate-Total-Cost-Performer/Data/Invoices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P15\Documents\UiPath\Calculate-Total-Cost\Calculate-Total-Cost-Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8002A5-79FC-4A5A-BD62-4818750C2700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5767FBB4-9E70-4E60-8B59-018C7B214C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10728" yWindow="2820" windowWidth="12312" windowHeight="9420" xr2:uid="{09F9C20C-53FB-447F-B91D-8FF60BDA9470}"/>
+    <workbookView xWindow="10728" yWindow="2820" windowWidth="12312" windowHeight="9420" xr2:uid="{374C5A81-0385-4255-89B9-851D75D72319}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,124 +59,124 @@
     <t>GrandTotal</t>
   </si>
   <si>
-    <t>Invoice 109.pdf</t>
-  </si>
-  <si>
-    <t>Ram Farndell</t>
-  </si>
-  <si>
-    <t>Invoice 110.pdf</t>
-  </si>
-  <si>
-    <t>Keri Wreiford</t>
-  </si>
-  <si>
-    <t>Invoice 111.pdf</t>
-  </si>
-  <si>
-    <t>Orville Gerhardt</t>
-  </si>
-  <si>
-    <t>Invoice 112.pdf</t>
-  </si>
-  <si>
-    <t>Hamilton Skouling</t>
-  </si>
-  <si>
-    <t>Invoice 113.pdf</t>
-  </si>
-  <si>
-    <t>Garwin Slorach</t>
-  </si>
-  <si>
-    <t>Invoice 114.pdf</t>
-  </si>
-  <si>
-    <t>Boony Dumper</t>
-  </si>
-  <si>
-    <t>Invoice 115.pdf</t>
+    <t>Invoice 269.pdf</t>
+  </si>
+  <si>
+    <t>Ricardo Noice</t>
+  </si>
+  <si>
+    <t>Invoice 270.pdf</t>
+  </si>
+  <si>
+    <t>Sandye Wankel</t>
+  </si>
+  <si>
+    <t>Invoice 271.pdf</t>
+  </si>
+  <si>
+    <t>Hagan Ledwitch</t>
+  </si>
+  <si>
+    <t>Invoice 272.pdf</t>
+  </si>
+  <si>
+    <t>Gale Yelland</t>
+  </si>
+  <si>
+    <t>Invoice 273.pdf</t>
+  </si>
+  <si>
+    <t>Marcelo Dewan</t>
+  </si>
+  <si>
+    <t>Invoice 274.pdf</t>
+  </si>
+  <si>
+    <t>Lena Hughes</t>
+  </si>
+  <si>
+    <t>Invoice 275.pdf</t>
   </si>
   <si>
     <t>Dulci Scay</t>
   </si>
   <si>
-    <t>Invoice 116.pdf</t>
-  </si>
-  <si>
-    <t>Keri Dancy</t>
-  </si>
-  <si>
-    <t>Invoice 117.pdf</t>
-  </si>
-  <si>
-    <t>Hamel Pavic</t>
-  </si>
-  <si>
-    <t>Invoice 118.pdf</t>
-  </si>
-  <si>
-    <t>Yancy Bulbrook</t>
-  </si>
-  <si>
-    <t>Invoice 119.pdf</t>
-  </si>
-  <si>
-    <t>Stirling Grunwald</t>
-  </si>
-  <si>
-    <t>Invoice 120.pdf</t>
-  </si>
-  <si>
-    <t>Wye Caseri</t>
-  </si>
-  <si>
-    <t>Invoice 121.pdf</t>
-  </si>
-  <si>
-    <t>Noby Everington</t>
-  </si>
-  <si>
-    <t>Invoice 122.pdf</t>
-  </si>
-  <si>
-    <t>Zorina Conibere</t>
-  </si>
-  <si>
-    <t>Invoice 123.pdf</t>
-  </si>
-  <si>
-    <t>Bridie Farbrace</t>
-  </si>
-  <si>
-    <t>Invoice 124.pdf</t>
-  </si>
-  <si>
-    <t>Zenia Beals</t>
-  </si>
-  <si>
-    <t>Invoice 125.pdf</t>
-  </si>
-  <si>
-    <t>Lynelle Vischi</t>
-  </si>
-  <si>
-    <t>Invoice 126.pdf</t>
-  </si>
-  <si>
-    <t>Jaquelyn De</t>
-  </si>
-  <si>
-    <t>Invoice 127.pdf</t>
-  </si>
-  <si>
-    <t>Dal Cremins</t>
-  </si>
-  <si>
-    <t>Invoice 128.pdf</t>
-  </si>
-  <si>
-    <t>Krissy Linney</t>
+    <t>Invoice 276.pdf</t>
+  </si>
+  <si>
+    <t>Karlen Gavin</t>
+  </si>
+  <si>
+    <t>Invoice 277.pdf</t>
+  </si>
+  <si>
+    <t>Marjie De</t>
+  </si>
+  <si>
+    <t>Invoice 278.pdf</t>
+  </si>
+  <si>
+    <t>Sianna Lavrinov</t>
+  </si>
+  <si>
+    <t>Invoice 279.pdf</t>
+  </si>
+  <si>
+    <t>Mycah McIver</t>
+  </si>
+  <si>
+    <t>Invoice 280.pdf</t>
+  </si>
+  <si>
+    <t>Manon Yele</t>
+  </si>
+  <si>
+    <t>Invoice 281.pdf</t>
+  </si>
+  <si>
+    <t>Priscella Paireman</t>
+  </si>
+  <si>
+    <t>Invoice 282.pdf</t>
+  </si>
+  <si>
+    <t>Stormie Nazair</t>
+  </si>
+  <si>
+    <t>Invoice 283.pdf</t>
+  </si>
+  <si>
+    <t>Tiebout Gatenby</t>
+  </si>
+  <si>
+    <t>Invoice 284.pdf</t>
+  </si>
+  <si>
+    <t>Bea Dyte</t>
+  </si>
+  <si>
+    <t>Invoice 285.pdf</t>
+  </si>
+  <si>
+    <t>Sancho Roxbee</t>
+  </si>
+  <si>
+    <t>Invoice 286.pdf</t>
+  </si>
+  <si>
+    <t>Wildon Brampton</t>
+  </si>
+  <si>
+    <t>Invoice 287.pdf</t>
+  </si>
+  <si>
+    <t>Marketa Soeiro</t>
+  </si>
+  <si>
+    <t>Invoice 288.pdf</t>
+  </si>
+  <si>
+    <t>Cassius Cassley</t>
   </si>
 </sst>
 </file>
@@ -561,7 +561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A8DB93-7D33-4594-B371-1626844A8EC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D316C7-1A9E-491E-8D8A-31D9C490FE0A}">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -605,22 +605,22 @@
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>42652</v>
+        <v>42599</v>
       </c>
       <c r="C2">
-        <v>6604</v>
+        <v>5004</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2">
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="F2">
-        <v>375</v>
+        <v>600</v>
       </c>
       <c r="G2">
-        <v>2375</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -628,22 +628,22 @@
         <v>9</v>
       </c>
       <c r="B3" s="1">
-        <v>42757</v>
+        <v>43246</v>
       </c>
       <c r="C3">
-        <v>3152</v>
+        <v>7953</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>1400</v>
+        <v>600</v>
       </c>
       <c r="F3">
-        <v>300</v>
+        <v>450</v>
       </c>
       <c r="G3">
-        <v>1700</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -651,22 +651,22 @@
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>43184</v>
+        <v>42542</v>
       </c>
       <c r="C4">
-        <v>6374</v>
+        <v>5556</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4">
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="F4">
         <v>675</v>
       </c>
       <c r="G4">
-        <v>1875</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -674,22 +674,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>43396</v>
+        <v>42930</v>
       </c>
       <c r="C5">
-        <v>9020</v>
+        <v>7232</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5">
-        <v>1200</v>
+        <v>400</v>
       </c>
       <c r="F5">
-        <v>450</v>
+        <v>750</v>
       </c>
       <c r="G5">
-        <v>1650</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -697,22 +697,22 @@
         <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>42696</v>
+        <v>42711</v>
       </c>
       <c r="C6">
-        <v>7008</v>
+        <v>4425</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="E6">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="F6">
         <v>300</v>
       </c>
       <c r="G6">
-        <v>900</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -720,22 +720,22 @@
         <v>17</v>
       </c>
       <c r="B7" s="1">
-        <v>43130</v>
+        <v>43036</v>
       </c>
       <c r="C7">
-        <v>5352</v>
+        <v>7181</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="F7">
-        <v>75</v>
+        <v>675</v>
       </c>
       <c r="G7">
-        <v>475</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -743,22 +743,22 @@
         <v>19</v>
       </c>
       <c r="B8" s="1">
-        <v>42671</v>
+        <v>43176</v>
       </c>
       <c r="C8">
-        <v>5255</v>
+        <v>5242</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
       <c r="E8">
-        <v>1400</v>
+        <v>200</v>
       </c>
       <c r="F8">
-        <v>600</v>
+        <v>675</v>
       </c>
       <c r="G8">
-        <v>2000</v>
+        <v>875</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -766,22 +766,22 @@
         <v>21</v>
       </c>
       <c r="B9" s="1">
-        <v>42665</v>
+        <v>42640</v>
       </c>
       <c r="C9">
-        <v>5402</v>
+        <v>7397</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
       </c>
       <c r="E9">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="F9">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="G9">
-        <v>1150</v>
+        <v>900</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -789,22 +789,22 @@
         <v>23</v>
       </c>
       <c r="B10" s="1">
-        <v>42632</v>
+        <v>42372</v>
       </c>
       <c r="C10">
-        <v>1443</v>
+        <v>3823</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
       </c>
       <c r="E10">
-        <v>1600</v>
+        <v>600</v>
       </c>
       <c r="F10">
-        <v>375</v>
+        <v>450</v>
       </c>
       <c r="G10">
-        <v>1975</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -812,22 +812,22 @@
         <v>25</v>
       </c>
       <c r="B11" s="1">
-        <v>42600</v>
+        <v>43268</v>
       </c>
       <c r="C11">
-        <v>5298</v>
+        <v>6235</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
       </c>
       <c r="E11">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="F11">
-        <v>225</v>
+        <v>525</v>
       </c>
       <c r="G11">
-        <v>1025</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -835,22 +835,22 @@
         <v>27</v>
       </c>
       <c r="B12" s="1">
-        <v>42891</v>
+        <v>43445</v>
       </c>
       <c r="C12">
-        <v>6357</v>
+        <v>1375</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
       </c>
       <c r="E12">
-        <v>400</v>
+        <v>1400</v>
       </c>
       <c r="F12">
-        <v>750</v>
+        <v>375</v>
       </c>
       <c r="G12">
-        <v>1150</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -858,22 +858,22 @@
         <v>29</v>
       </c>
       <c r="B13" s="1">
-        <v>42664</v>
+        <v>43329</v>
       </c>
       <c r="C13">
-        <v>3893</v>
+        <v>4072</v>
       </c>
       <c r="D13" t="s">
         <v>30</v>
       </c>
       <c r="E13">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F13">
-        <v>525</v>
+        <v>300</v>
       </c>
       <c r="G13">
-        <v>925</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -881,22 +881,22 @@
         <v>31</v>
       </c>
       <c r="B14" s="1">
-        <v>42483</v>
+        <v>42453</v>
       </c>
       <c r="C14">
-        <v>7260</v>
+        <v>6656</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
       </c>
       <c r="E14">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="F14">
-        <v>300</v>
+        <v>675</v>
       </c>
       <c r="G14">
-        <v>2300</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -904,22 +904,22 @@
         <v>33</v>
       </c>
       <c r="B15" s="1">
-        <v>42946</v>
+        <v>43406</v>
       </c>
       <c r="C15">
-        <v>2381</v>
+        <v>1191</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
       </c>
       <c r="E15">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="F15">
         <v>450</v>
       </c>
       <c r="G15">
-        <v>2050</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -927,10 +927,10 @@
         <v>35</v>
       </c>
       <c r="B16" s="1">
-        <v>43094</v>
+        <v>42905</v>
       </c>
       <c r="C16">
-        <v>5542</v>
+        <v>6376</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -939,10 +939,10 @@
         <v>1000</v>
       </c>
       <c r="F16">
-        <v>525</v>
+        <v>375</v>
       </c>
       <c r="G16">
-        <v>1525</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -950,22 +950,22 @@
         <v>37</v>
       </c>
       <c r="B17" s="1">
-        <v>43434</v>
+        <v>43456</v>
       </c>
       <c r="C17">
-        <v>8437</v>
+        <v>2264</v>
       </c>
       <c r="D17" t="s">
         <v>38</v>
       </c>
       <c r="E17">
-        <v>1400</v>
+        <v>200</v>
       </c>
       <c r="F17">
-        <v>75</v>
+        <v>600</v>
       </c>
       <c r="G17">
-        <v>1475</v>
+        <v>800</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -973,22 +973,22 @@
         <v>39</v>
       </c>
       <c r="B18" s="1">
-        <v>42386</v>
+        <v>42936</v>
       </c>
       <c r="C18">
-        <v>7354</v>
+        <v>5789</v>
       </c>
       <c r="D18" t="s">
         <v>40</v>
       </c>
       <c r="E18">
-        <v>1600</v>
+        <v>400</v>
       </c>
       <c r="F18">
-        <v>150</v>
+        <v>375</v>
       </c>
       <c r="G18">
-        <v>1750</v>
+        <v>775</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -996,22 +996,22 @@
         <v>41</v>
       </c>
       <c r="B19" s="1">
-        <v>42425</v>
+        <v>42721</v>
       </c>
       <c r="C19">
-        <v>5424</v>
+        <v>5873</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
       </c>
       <c r="E19">
-        <v>1400</v>
+        <v>200</v>
       </c>
       <c r="F19">
         <v>600</v>
       </c>
       <c r="G19">
-        <v>2000</v>
+        <v>800</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1019,22 +1019,22 @@
         <v>43</v>
       </c>
       <c r="B20" s="1">
-        <v>43054</v>
+        <v>43285</v>
       </c>
       <c r="C20">
-        <v>8179</v>
+        <v>8257</v>
       </c>
       <c r="D20" t="s">
         <v>44</v>
       </c>
       <c r="E20">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="F20">
-        <v>450</v>
+        <v>225</v>
       </c>
       <c r="G20">
-        <v>2050</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1042,22 +1042,22 @@
         <v>45</v>
       </c>
       <c r="B21" s="1">
-        <v>43249</v>
+        <v>43177</v>
       </c>
       <c r="C21">
-        <v>7189</v>
+        <v>8084</v>
       </c>
       <c r="D21" t="s">
         <v>46</v>
       </c>
       <c r="E21">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="F21">
-        <v>525</v>
+        <v>750</v>
       </c>
       <c r="G21">
-        <v>1525</v>
+        <v>2550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>